<commit_message>
🚀 Successfully npm run build
</commit_message>
<xml_diff>
--- a/script/sample.xlsx
+++ b/script/sample.xlsx
@@ -593,13 +593,41 @@
           <t>['Sample Markdown']</t>
         </is>
       </c>
-      <c r="L2" t="inlineStr"/>
-      <c r="M2" t="inlineStr"/>
-      <c r="N2" t="inlineStr"/>
-      <c r="O2" t="inlineStr"/>
-      <c r="P2" t="inlineStr"/>
-      <c r="Q2" t="inlineStr"/>
-      <c r="R2" t="inlineStr"/>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="S2" t="inlineStr">
         <is>
           <t>Shoto Morisaki</t>
@@ -607,7 +635,7 @@
       </c>
       <c r="T2" t="inlineStr">
         <is>
-          <t>[{'icon': 'fab fa-facebook-f', 'url': None}, {'icon': 'fa-brands fa-x-twitter', 'url': None}, {'icon': 'fas fa-link', 'url': None}]</t>
+          <t>[{'icon': 'fab fa-facebook-f', 'url': 'None'}, {'icon': 'fa-brands fa-x-twitter', 'url': 'None'}, {'icon': 'fas fa-link', 'url': 'None'}]</t>
         </is>
       </c>
     </row>
@@ -667,13 +695,41 @@
           <t>['LLM', 'Natural Language', 'LangChain', 'RAG']</t>
         </is>
       </c>
-      <c r="L3" t="inlineStr"/>
-      <c r="M3" t="inlineStr"/>
-      <c r="N3" t="inlineStr"/>
-      <c r="O3" t="inlineStr"/>
-      <c r="P3" t="inlineStr"/>
-      <c r="Q3" t="inlineStr"/>
-      <c r="R3" t="inlineStr"/>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="S3" t="inlineStr">
         <is>
           <t>Shoto Morisaki</t>
@@ -681,7 +737,7 @@
       </c>
       <c r="T3" t="inlineStr">
         <is>
-          <t>[{'icon': 'fab fa-facebook-f', 'url': None}, {'icon': 'fa-brands fa-x-twitter', 'url': None}, {'icon': 'fas fa-link', 'url': None}]</t>
+          <t>[{'icon': 'fab fa-facebook-f', 'url': 'None'}, {'icon': 'fa-brands fa-x-twitter', 'url': 'None'}, {'icon': 'fas fa-link', 'url': 'None'}]</t>
         </is>
       </c>
     </row>
@@ -741,13 +797,41 @@
           <t>['AWS', 'Docker', 'Python Flask', 'Material-UI', 'ApexCharts', 'TypeScript', 'React']</t>
         </is>
       </c>
-      <c r="L4" t="inlineStr"/>
-      <c r="M4" t="inlineStr"/>
-      <c r="N4" t="inlineStr"/>
-      <c r="O4" t="inlineStr"/>
-      <c r="P4" t="inlineStr"/>
-      <c r="Q4" t="inlineStr"/>
-      <c r="R4" t="inlineStr"/>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="S4" t="inlineStr">
         <is>
           <t>Shoto Morisaki</t>
@@ -755,7 +839,7 @@
       </c>
       <c r="T4" t="inlineStr">
         <is>
-          <t>[{'icon': 'fab fa-facebook-f', 'url': None}, {'icon': 'fa-brands fa-x-twitter', 'url': None}, {'icon': 'fas fa-link', 'url': None}]</t>
+          <t>[{'icon': 'fab fa-facebook-f', 'url': 'None'}, {'icon': 'fa-brands fa-x-twitter', 'url': 'None'}, {'icon': 'fas fa-link', 'url': 'None'}]</t>
         </is>
       </c>
     </row>
@@ -813,13 +897,41 @@
           <t>['Internship', 'Software Engineering']</t>
         </is>
       </c>
-      <c r="L5" t="inlineStr"/>
-      <c r="M5" t="inlineStr"/>
-      <c r="N5" t="inlineStr"/>
-      <c r="O5" t="inlineStr"/>
-      <c r="P5" t="inlineStr"/>
-      <c r="Q5" t="inlineStr"/>
-      <c r="R5" t="inlineStr"/>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="S5" t="inlineStr">
         <is>
           <t>Shoto Morisaki</t>
@@ -827,7 +939,7 @@
       </c>
       <c r="T5" t="inlineStr">
         <is>
-          <t>[{'icon': 'fab fa-facebook-f', 'url': None}, {'icon': 'fa-brands fa-x-twitter', 'url': None}, {'icon': 'fas fa-link', 'url': None}]</t>
+          <t>[{'icon': 'fab fa-facebook-f', 'url': 'None'}, {'icon': 'fa-brands fa-x-twitter', 'url': 'None'}, {'icon': 'fas fa-link', 'url': 'None'}]</t>
         </is>
       </c>
     </row>
@@ -887,13 +999,41 @@
           <t>['RESTfulAPI', 'React', 'Typescript', 'GPTAPI', 'HuggingFaceModel']</t>
         </is>
       </c>
-      <c r="L6" t="inlineStr"/>
-      <c r="M6" t="inlineStr"/>
-      <c r="N6" t="inlineStr"/>
-      <c r="O6" t="inlineStr"/>
-      <c r="P6" t="inlineStr"/>
-      <c r="Q6" t="inlineStr"/>
-      <c r="R6" t="inlineStr"/>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="S6" t="inlineStr">
         <is>
           <t>Shoto Morisaki</t>
@@ -901,7 +1041,7 @@
       </c>
       <c r="T6" t="inlineStr">
         <is>
-          <t>[{'icon': 'fab fa-facebook-f', 'url': None}, {'icon': 'fa-brands fa-x-twitter', 'url': None}, {'icon': 'fas fa-link', 'url': None}]</t>
+          <t>[{'icon': 'fab fa-facebook-f', 'url': 'None'}, {'icon': 'fa-brands fa-x-twitter', 'url': 'None'}, {'icon': 'fas fa-link', 'url': 'None'}]</t>
         </is>
       </c>
     </row>
@@ -961,13 +1101,41 @@
           <t>['Internship', 'LLM', 'Natural Language', 'RAG']</t>
         </is>
       </c>
-      <c r="L7" t="inlineStr"/>
-      <c r="M7" t="inlineStr"/>
-      <c r="N7" t="inlineStr"/>
-      <c r="O7" t="inlineStr"/>
-      <c r="P7" t="inlineStr"/>
-      <c r="Q7" t="inlineStr"/>
-      <c r="R7" t="inlineStr"/>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="S7" t="inlineStr">
         <is>
           <t>Shoto Morisaki</t>
@@ -975,7 +1143,7 @@
       </c>
       <c r="T7" t="inlineStr">
         <is>
-          <t>[{'icon': 'fab fa-facebook-f', 'url': None}, {'icon': 'fa-brands fa-x-twitter', 'url': None}, {'icon': 'fas fa-link', 'url': None}]</t>
+          <t>[{'icon': 'fab fa-facebook-f', 'url': 'None'}, {'icon': 'fa-brands fa-x-twitter', 'url': 'None'}, {'icon': 'fas fa-link', 'url': 'None'}]</t>
         </is>
       </c>
     </row>
@@ -1035,13 +1203,41 @@
           <t>['FastAPI', 'Flask', 'GPT API']</t>
         </is>
       </c>
-      <c r="L8" t="inlineStr"/>
-      <c r="M8" t="inlineStr"/>
-      <c r="N8" t="inlineStr"/>
-      <c r="O8" t="inlineStr"/>
-      <c r="P8" t="inlineStr"/>
-      <c r="Q8" t="inlineStr"/>
-      <c r="R8" t="inlineStr"/>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="R8" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="S8" t="inlineStr">
         <is>
           <t>Shoto Morisaki</t>
@@ -1049,7 +1245,7 @@
       </c>
       <c r="T8" t="inlineStr">
         <is>
-          <t>[{'icon': 'fab fa-facebook-f', 'url': None}, {'icon': 'fa-brands fa-x-twitter', 'url': None}, {'icon': 'fas fa-link', 'url': None}]</t>
+          <t>[{'icon': 'fab fa-facebook-f', 'url': 'None'}, {'icon': 'fa-brands fa-x-twitter', 'url': 'None'}, {'icon': 'fas fa-link', 'url': 'None'}]</t>
         </is>
       </c>
     </row>
@@ -1084,10 +1280,8 @@
           <t>README_for_team</t>
         </is>
       </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>2024-02-24</t>
-        </is>
+      <c r="G9" s="2" t="n">
+        <v>45346</v>
       </c>
       <c r="H9" t="inlineStr">
         <is>
@@ -1109,13 +1303,41 @@
           <t>['Coding', 'README']</t>
         </is>
       </c>
-      <c r="L9" t="inlineStr"/>
-      <c r="M9" t="inlineStr"/>
-      <c r="N9" t="inlineStr"/>
-      <c r="O9" t="inlineStr"/>
-      <c r="P9" t="inlineStr"/>
-      <c r="Q9" t="inlineStr"/>
-      <c r="R9" t="inlineStr"/>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="P9" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="Q9" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="R9" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="S9" t="inlineStr">
         <is>
           <t>Shoto Morisaki</t>
@@ -1123,7 +1345,7 @@
       </c>
       <c r="T9" t="inlineStr">
         <is>
-          <t>[{'icon': 'fab fa-facebook-f', 'url': None}, {'icon': 'fa-brands fa-x-twitter', 'url': None}, {'icon': 'fas fa-link', 'url': None}]</t>
+          <t>[{'icon': 'fab fa-facebook-f', 'url': 'None'}, {'icon': 'fa-brands fa-x-twitter', 'url': 'None'}, {'icon': 'fas fa-link', 'url': 'None'}]</t>
         </is>
       </c>
     </row>
@@ -1181,13 +1403,41 @@
           <t>['Large Language Models', 'Hallucination Mitigation', 'Techniques', 'Survey']</t>
         </is>
       </c>
-      <c r="L10" t="inlineStr"/>
-      <c r="M10" t="inlineStr"/>
-      <c r="N10" t="inlineStr"/>
-      <c r="O10" t="inlineStr"/>
-      <c r="P10" t="inlineStr"/>
-      <c r="Q10" t="inlineStr"/>
-      <c r="R10" t="inlineStr"/>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="P10" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="R10" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="S10" t="inlineStr">
         <is>
           <t>Shoto Morisaki</t>
@@ -1195,14 +1445,14 @@
       </c>
       <c r="T10" t="inlineStr">
         <is>
-          <t>[{'icon': 'fab fa-facebook-f', 'url': None}, {'icon': 'fa-brands fa-x-twitter', 'url': None}, {'icon': 'fas fa-link', 'url': None}]</t>
+          <t>[{'icon': 'fab fa-facebook-f', 'url': 'None'}, {'icon': 'fa-brands fa-x-twitter', 'url': 'None'}, {'icon': 'fas fa-link', 'url': 'None'}]</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Published</t>
+          <t>Draft</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -1255,13 +1505,41 @@
           <t>['Coding', 'README']</t>
         </is>
       </c>
-      <c r="L11" t="inlineStr"/>
-      <c r="M11" t="inlineStr"/>
-      <c r="N11" t="inlineStr"/>
-      <c r="O11" t="inlineStr"/>
-      <c r="P11" t="inlineStr"/>
-      <c r="Q11" t="inlineStr"/>
-      <c r="R11" t="inlineStr"/>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="P11" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="Q11" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="R11" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="S11" t="inlineStr">
         <is>
           <t>Shoto Morisaki</t>
@@ -1269,7 +1547,7 @@
       </c>
       <c r="T11" t="inlineStr">
         <is>
-          <t>[{'icon': 'fab fa-facebook-f', 'url': None}, {'icon': 'fa-brands fa-x-twitter', 'url': None}, {'icon': 'fas fa-link', 'url': None}]</t>
+          <t>[{'icon': 'fab fa-facebook-f', 'url': 'None'}, {'icon': 'fa-brands fa-x-twitter', 'url': 'None'}, {'icon': 'fas fa-link', 'url': 'None'}]</t>
         </is>
       </c>
     </row>
@@ -1304,10 +1582,8 @@
           <t>Hackathon_Startup 101</t>
         </is>
       </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>2024-04-10</t>
-        </is>
+      <c r="G12" s="2" t="n">
+        <v>45392</v>
       </c>
       <c r="H12" t="inlineStr">
         <is>
@@ -1329,13 +1605,41 @@
           <t>['Hackathon', 'Startup', 'Idea Matters']</t>
         </is>
       </c>
-      <c r="L12" t="inlineStr"/>
-      <c r="M12" t="inlineStr"/>
-      <c r="N12" t="inlineStr"/>
-      <c r="O12" t="inlineStr"/>
-      <c r="P12" t="inlineStr"/>
-      <c r="Q12" t="inlineStr"/>
-      <c r="R12" t="inlineStr"/>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="P12" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="Q12" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="R12" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="S12" t="inlineStr">
         <is>
           <t>Shoto Morisaki</t>
@@ -1343,7 +1647,7 @@
       </c>
       <c r="T12" t="inlineStr">
         <is>
-          <t>[{'icon': 'fab fa-facebook-f', 'url': None}, {'icon': 'fa-brands fa-x-twitter', 'url': None}, {'icon': 'fas fa-link', 'url': None}]</t>
+          <t>[{'icon': 'fab fa-facebook-f', 'url': 'None'}, {'icon': 'fa-brands fa-x-twitter', 'url': 'None'}, {'icon': 'fas fa-link', 'url': 'None'}]</t>
         </is>
       </c>
     </row>
@@ -1403,13 +1707,41 @@
           <t>['Hackathon', 'LLM', 'Law', 'RAG']</t>
         </is>
       </c>
-      <c r="L13" t="inlineStr"/>
-      <c r="M13" t="inlineStr"/>
-      <c r="N13" t="inlineStr"/>
-      <c r="O13" t="inlineStr"/>
-      <c r="P13" t="inlineStr"/>
-      <c r="Q13" t="inlineStr"/>
-      <c r="R13" t="inlineStr"/>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="P13" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="Q13" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="R13" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="S13" t="inlineStr">
         <is>
           <t>Shoto Morisaki</t>
@@ -1417,7 +1749,7 @@
       </c>
       <c r="T13" t="inlineStr">
         <is>
-          <t>[{'icon': 'fab fa-facebook-f', 'url': None}, {'icon': 'fa-brands fa-x-twitter', 'url': None}, {'icon': 'fas fa-link', 'url': None}]</t>
+          <t>[{'icon': 'fab fa-facebook-f', 'url': 'None'}, {'icon': 'fa-brands fa-x-twitter', 'url': 'None'}, {'icon': 'fas fa-link', 'url': 'None'}]</t>
         </is>
       </c>
     </row>
@@ -1477,13 +1809,41 @@
           <t>['Flutter', '3DModel', 'GoogleMapAPI', 'LumaAPI']</t>
         </is>
       </c>
-      <c r="L14" t="inlineStr"/>
-      <c r="M14" t="inlineStr"/>
-      <c r="N14" t="inlineStr"/>
-      <c r="O14" t="inlineStr"/>
-      <c r="P14" t="inlineStr"/>
-      <c r="Q14" t="inlineStr"/>
-      <c r="R14" t="inlineStr"/>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="P14" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="Q14" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="R14" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="S14" t="inlineStr">
         <is>
           <t>Shoto Morisaki</t>
@@ -1491,7 +1851,7 @@
       </c>
       <c r="T14" t="inlineStr">
         <is>
-          <t>[{'icon': 'fab fa-facebook-f', 'url': None}, {'icon': 'fa-brands fa-x-twitter', 'url': None}, {'icon': 'fas fa-link', 'url': None}]</t>
+          <t>[{'icon': 'fab fa-facebook-f', 'url': 'None'}, {'icon': 'fa-brands fa-x-twitter', 'url': 'None'}, {'icon': 'fas fa-link', 'url': 'None'}]</t>
         </is>
       </c>
     </row>
@@ -1551,13 +1911,41 @@
           <t>['RAG', 'LLM', 'Knowledge Injection', 'Fine-tuning', 'External Data']</t>
         </is>
       </c>
-      <c r="L15" t="inlineStr"/>
-      <c r="M15" t="inlineStr"/>
-      <c r="N15" t="inlineStr"/>
-      <c r="O15" t="inlineStr"/>
-      <c r="P15" t="inlineStr"/>
-      <c r="Q15" t="inlineStr"/>
-      <c r="R15" t="inlineStr"/>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="P15" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="Q15" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="R15" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="S15" t="inlineStr">
         <is>
           <t>Shoto Morisaki</t>
@@ -1565,7 +1953,7 @@
       </c>
       <c r="T15" t="inlineStr">
         <is>
-          <t>[{'icon': 'fab fa-facebook-f', 'url': None}, {'icon': 'fa-brands fa-x-twitter', 'url': None}, {'icon': 'fas fa-link', 'url': None}]</t>
+          <t>[{'icon': 'fab fa-facebook-f', 'url': 'None'}, {'icon': 'fa-brands fa-x-twitter', 'url': 'None'}, {'icon': 'fas fa-link', 'url': 'None'}]</t>
         </is>
       </c>
     </row>
@@ -1625,13 +2013,41 @@
           <t>['Research', 'Cybersecurity']</t>
         </is>
       </c>
-      <c r="L16" t="inlineStr"/>
-      <c r="M16" t="inlineStr"/>
-      <c r="N16" t="inlineStr"/>
-      <c r="O16" t="inlineStr"/>
-      <c r="P16" t="inlineStr"/>
-      <c r="Q16" t="inlineStr"/>
-      <c r="R16" t="inlineStr"/>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="O16" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="P16" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="Q16" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="R16" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="S16" t="inlineStr">
         <is>
           <t>Shoto Morisaki</t>
@@ -1639,7 +2055,7 @@
       </c>
       <c r="T16" t="inlineStr">
         <is>
-          <t>[{'icon': 'fab fa-facebook-f', 'url': None}, {'icon': 'fa-brands fa-x-twitter', 'url': None}, {'icon': 'fas fa-link', 'url': None}]</t>
+          <t>[{'icon': 'fab fa-facebook-f', 'url': 'None'}, {'icon': 'fa-brands fa-x-twitter', 'url': 'None'}, {'icon': 'fas fa-link', 'url': 'None'}]</t>
         </is>
       </c>
     </row>
@@ -1697,13 +2113,41 @@
           <t>['Git']</t>
         </is>
       </c>
-      <c r="L17" t="inlineStr"/>
-      <c r="M17" t="inlineStr"/>
-      <c r="N17" t="inlineStr"/>
-      <c r="O17" t="inlineStr"/>
-      <c r="P17" t="inlineStr"/>
-      <c r="Q17" t="inlineStr"/>
-      <c r="R17" t="inlineStr"/>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="O17" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="P17" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="Q17" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="R17" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="S17" t="inlineStr">
         <is>
           <t>Shoto Morisaki</t>
@@ -1711,7 +2155,7 @@
       </c>
       <c r="T17" t="inlineStr">
         <is>
-          <t>[{'icon': 'fab fa-facebook-f', 'url': None}, {'icon': 'fa-brands fa-x-twitter', 'url': None}, {'icon': 'fas fa-link', 'url': None}]</t>
+          <t>[{'icon': 'fab fa-facebook-f', 'url': 'None'}, {'icon': 'fa-brands fa-x-twitter', 'url': 'None'}, {'icon': 'fas fa-link', 'url': 'None'}]</t>
         </is>
       </c>
     </row>
@@ -1769,13 +2213,41 @@
           <t>['Git']</t>
         </is>
       </c>
-      <c r="L18" t="inlineStr"/>
-      <c r="M18" t="inlineStr"/>
-      <c r="N18" t="inlineStr"/>
-      <c r="O18" t="inlineStr"/>
-      <c r="P18" t="inlineStr"/>
-      <c r="Q18" t="inlineStr"/>
-      <c r="R18" t="inlineStr"/>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="O18" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="P18" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="Q18" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="R18" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="S18" t="inlineStr">
         <is>
           <t>Shoto Morisaki</t>
@@ -1783,7 +2255,7 @@
       </c>
       <c r="T18" t="inlineStr">
         <is>
-          <t>[{'icon': 'fab fa-facebook-f', 'url': None}, {'icon': 'fa-brands fa-x-twitter', 'url': None}, {'icon': 'fas fa-link', 'url': None}]</t>
+          <t>[{'icon': 'fab fa-facebook-f', 'url': 'None'}, {'icon': 'fa-brands fa-x-twitter', 'url': 'None'}, {'icon': 'fas fa-link', 'url': 'None'}]</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
✨ Making base lien
</commit_message>
<xml_diff>
--- a/script/sample.xlsx
+++ b/script/sample.xlsx
@@ -600,7 +600,7 @@
       <c r="P2" t="inlineStr"/>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>https://github.com/shoot649854/IMG_DB/blob/main/profile.webp</t>
+          <t>https://raw.githubusercontent.com/shoot649854/IMG_DB/main/profile.webp</t>
         </is>
       </c>
       <c r="R2" t="inlineStr">
@@ -682,7 +682,7 @@
       <c r="P3" t="inlineStr"/>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>https://github.com/shoot649854/IMG_DB/blob/main/profile.webp</t>
+          <t>https://raw.githubusercontent.com/shoot649854/IMG_DB/main/profile.webp</t>
         </is>
       </c>
       <c r="R3" t="inlineStr">
@@ -764,7 +764,7 @@
       <c r="P4" t="inlineStr"/>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>https://github.com/shoot649854/IMG_DB/blob/main/profile.webp</t>
+          <t>https://raw.githubusercontent.com/shoot649854/IMG_DB/main/profile.webp</t>
         </is>
       </c>
       <c r="R4" t="inlineStr">
@@ -844,7 +844,7 @@
       <c r="P5" t="inlineStr"/>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>https://github.com/shoot649854/IMG_DB/blob/main/profile.webp</t>
+          <t>https://raw.githubusercontent.com/shoot649854/IMG_DB/main/profile.webp</t>
         </is>
       </c>
       <c r="R5" t="inlineStr">
@@ -926,7 +926,7 @@
       <c r="P6" t="inlineStr"/>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>https://github.com/shoot649854/IMG_DB/blob/main/profile.webp</t>
+          <t>https://raw.githubusercontent.com/shoot649854/IMG_DB/main/profile.webp</t>
         </is>
       </c>
       <c r="R6" t="inlineStr">
@@ -1008,7 +1008,7 @@
       <c r="P7" t="inlineStr"/>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>https://github.com/shoot649854/IMG_DB/blob/main/profile.webp</t>
+          <t>https://raw.githubusercontent.com/shoot649854/IMG_DB/main/profile.webp</t>
         </is>
       </c>
       <c r="R7" t="inlineStr">
@@ -1090,7 +1090,7 @@
       <c r="P8" t="inlineStr"/>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>https://github.com/shoot649854/IMG_DB/blob/main/profile.webp</t>
+          <t>https://raw.githubusercontent.com/shoot649854/IMG_DB/main/profile.webp</t>
         </is>
       </c>
       <c r="R8" t="inlineStr">
@@ -1170,7 +1170,7 @@
       <c r="P9" t="inlineStr"/>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>https://github.com/shoot649854/IMG_DB/blob/main/profile.webp</t>
+          <t>https://raw.githubusercontent.com/shoot649854/IMG_DB/main/profile.webp</t>
         </is>
       </c>
       <c r="R9" t="inlineStr">
@@ -1250,7 +1250,7 @@
       <c r="P10" t="inlineStr"/>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>https://github.com/shoot649854/IMG_DB/blob/main/profile.webp</t>
+          <t>https://raw.githubusercontent.com/shoot649854/IMG_DB/main/profile.webp</t>
         </is>
       </c>
       <c r="R10" t="inlineStr">
@@ -1332,7 +1332,7 @@
       <c r="P11" t="inlineStr"/>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>https://github.com/shoot649854/IMG_DB/blob/main/profile.webp</t>
+          <t>https://raw.githubusercontent.com/shoot649854/IMG_DB/main/profile.webp</t>
         </is>
       </c>
       <c r="R11" t="inlineStr">
@@ -1412,7 +1412,7 @@
       <c r="P12" t="inlineStr"/>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>https://github.com/shoot649854/IMG_DB/blob/main/profile.webp</t>
+          <t>https://raw.githubusercontent.com/shoot649854/IMG_DB/main/profile.webp</t>
         </is>
       </c>
       <c r="R12" t="inlineStr">
@@ -1494,7 +1494,7 @@
       <c r="P13" t="inlineStr"/>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>https://github.com/shoot649854/IMG_DB/blob/main/profile.webp</t>
+          <t>https://raw.githubusercontent.com/shoot649854/IMG_DB/main/profile.webp</t>
         </is>
       </c>
       <c r="R13" t="inlineStr">
@@ -1576,7 +1576,7 @@
       <c r="P14" t="inlineStr"/>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>https://github.com/shoot649854/IMG_DB/blob/main/profile.webp</t>
+          <t>https://raw.githubusercontent.com/shoot649854/IMG_DB/main/profile.webp</t>
         </is>
       </c>
       <c r="R14" t="inlineStr">
@@ -1658,7 +1658,7 @@
       <c r="P15" t="inlineStr"/>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>https://github.com/shoot649854/IMG_DB/blob/main/profile.webp</t>
+          <t>https://raw.githubusercontent.com/shoot649854/IMG_DB/main/profile.webp</t>
         </is>
       </c>
       <c r="R15" t="inlineStr">
@@ -1740,7 +1740,7 @@
       <c r="P16" t="inlineStr"/>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>https://github.com/shoot649854/IMG_DB/blob/main/profile.webp</t>
+          <t>https://raw.githubusercontent.com/shoot649854/IMG_DB/main/profile.webp</t>
         </is>
       </c>
       <c r="R16" t="inlineStr">
@@ -1820,7 +1820,7 @@
       <c r="P17" t="inlineStr"/>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>https://github.com/shoot649854/IMG_DB/blob/main/profile.webp</t>
+          <t>https://raw.githubusercontent.com/shoot649854/IMG_DB/main/profile.webp</t>
         </is>
       </c>
       <c r="R17" t="inlineStr">
@@ -1900,7 +1900,7 @@
       <c r="P18" t="inlineStr"/>
       <c r="Q18" t="inlineStr">
         <is>
-          <t>https://github.com/shoot649854/IMG_DB/blob/main/profile.webp</t>
+          <t>https://raw.githubusercontent.com/shoot649854/IMG_DB/main/profile.webp</t>
         </is>
       </c>
       <c r="R18" t="inlineStr">

</xml_diff>

<commit_message>
📝 Adding posts/17_Human_Factors_Formal_Methods and cleaning app files
</commit_message>
<xml_diff>
--- a/script/sample.xlsx
+++ b/script/sample.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T18"/>
+  <dimension ref="A1:T19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -600,7 +600,7 @@
       <c r="P2" t="inlineStr"/>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>https://github.com/shoot649854/IMG_DB/blob/main/profile.webp</t>
+          <t>https://raw.githubusercontent.com/shoot649854/IMG_DB/main/profile.webp</t>
         </is>
       </c>
       <c r="R2" t="inlineStr">
@@ -682,7 +682,7 @@
       <c r="P3" t="inlineStr"/>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>https://github.com/shoot649854/IMG_DB/blob/main/profile.webp</t>
+          <t>https://raw.githubusercontent.com/shoot649854/IMG_DB/main/profile.webp</t>
         </is>
       </c>
       <c r="R3" t="inlineStr">
@@ -754,7 +754,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>['AWS', 'Docker', 'Python Flask', 'Material-UI', 'ApexCharts', 'TypeScript', 'React']</t>
+          <t>['AWS', 'Docker', 'Python', 'Flask', 'MUI', 'TypeScript', 'React']</t>
         </is>
       </c>
       <c r="L4" t="inlineStr"/>
@@ -764,7 +764,7 @@
       <c r="P4" t="inlineStr"/>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>https://github.com/shoot649854/IMG_DB/blob/main/profile.webp</t>
+          <t>https://raw.githubusercontent.com/shoot649854/IMG_DB/main/profile.webp</t>
         </is>
       </c>
       <c r="R4" t="inlineStr">
@@ -844,7 +844,7 @@
       <c r="P5" t="inlineStr"/>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>https://github.com/shoot649854/IMG_DB/blob/main/profile.webp</t>
+          <t>https://raw.githubusercontent.com/shoot649854/IMG_DB/main/profile.webp</t>
         </is>
       </c>
       <c r="R5" t="inlineStr">
@@ -926,7 +926,7 @@
       <c r="P6" t="inlineStr"/>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>https://github.com/shoot649854/IMG_DB/blob/main/profile.webp</t>
+          <t>https://raw.githubusercontent.com/shoot649854/IMG_DB/main/profile.webp</t>
         </is>
       </c>
       <c r="R6" t="inlineStr">
@@ -1008,7 +1008,7 @@
       <c r="P7" t="inlineStr"/>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>https://github.com/shoot649854/IMG_DB/blob/main/profile.webp</t>
+          <t>https://raw.githubusercontent.com/shoot649854/IMG_DB/main/profile.webp</t>
         </is>
       </c>
       <c r="R7" t="inlineStr">
@@ -1090,7 +1090,7 @@
       <c r="P8" t="inlineStr"/>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>https://github.com/shoot649854/IMG_DB/blob/main/profile.webp</t>
+          <t>https://raw.githubusercontent.com/shoot649854/IMG_DB/main/profile.webp</t>
         </is>
       </c>
       <c r="R8" t="inlineStr">
@@ -1170,7 +1170,7 @@
       <c r="P9" t="inlineStr"/>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>https://github.com/shoot649854/IMG_DB/blob/main/profile.webp</t>
+          <t>https://raw.githubusercontent.com/shoot649854/IMG_DB/main/profile.webp</t>
         </is>
       </c>
       <c r="R9" t="inlineStr">
@@ -1250,7 +1250,7 @@
       <c r="P10" t="inlineStr"/>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>https://github.com/shoot649854/IMG_DB/blob/main/profile.webp</t>
+          <t>https://raw.githubusercontent.com/shoot649854/IMG_DB/main/profile.webp</t>
         </is>
       </c>
       <c r="R10" t="inlineStr">
@@ -1332,7 +1332,7 @@
       <c r="P11" t="inlineStr"/>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>https://github.com/shoot649854/IMG_DB/blob/main/profile.webp</t>
+          <t>https://raw.githubusercontent.com/shoot649854/IMG_DB/main/profile.webp</t>
         </is>
       </c>
       <c r="R11" t="inlineStr">
@@ -1412,7 +1412,7 @@
       <c r="P12" t="inlineStr"/>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>https://github.com/shoot649854/IMG_DB/blob/main/profile.webp</t>
+          <t>https://raw.githubusercontent.com/shoot649854/IMG_DB/main/profile.webp</t>
         </is>
       </c>
       <c r="R12" t="inlineStr">
@@ -1494,7 +1494,7 @@
       <c r="P13" t="inlineStr"/>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>https://github.com/shoot649854/IMG_DB/blob/main/profile.webp</t>
+          <t>https://raw.githubusercontent.com/shoot649854/IMG_DB/main/profile.webp</t>
         </is>
       </c>
       <c r="R13" t="inlineStr">
@@ -1576,7 +1576,7 @@
       <c r="P14" t="inlineStr"/>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>https://github.com/shoot649854/IMG_DB/blob/main/profile.webp</t>
+          <t>https://raw.githubusercontent.com/shoot649854/IMG_DB/main/profile.webp</t>
         </is>
       </c>
       <c r="R14" t="inlineStr">
@@ -1658,7 +1658,7 @@
       <c r="P15" t="inlineStr"/>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>https://github.com/shoot649854/IMG_DB/blob/main/profile.webp</t>
+          <t>https://raw.githubusercontent.com/shoot649854/IMG_DB/main/profile.webp</t>
         </is>
       </c>
       <c r="R15" t="inlineStr">
@@ -1740,7 +1740,7 @@
       <c r="P16" t="inlineStr"/>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>https://github.com/shoot649854/IMG_DB/blob/main/profile.webp</t>
+          <t>https://raw.githubusercontent.com/shoot649854/IMG_DB/main/profile.webp</t>
         </is>
       </c>
       <c r="R16" t="inlineStr">
@@ -1772,26 +1772,26 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>17</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Commonly Used React HooksGithub accounts</t>
+          <t>The Human Factors of Formal Methods</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>List of commonly used React hooks with brief explanations.</t>
+          <t>As formal methods improve in expressiveness and power, they create new opportunities for non-expert adoption. In principle, formal tools are now powerful enough to enable developers to scalably validate realistic systems artifacts without extensive formal training.</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>React_Hooks</t>
+          <t>Human_Factors_Formal_Methods</t>
         </is>
       </c>
       <c r="G17" s="2" t="n">
-        <v>45333</v>
+        <v>45399</v>
       </c>
       <c r="H17" t="inlineStr">
         <is>
@@ -1800,17 +1800,17 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>sample/opened-laptop.jpg</t>
+          <t>sample/sample7.jpg</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>Coding</t>
+          <t>Article</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>['Git']</t>
+          <t>['Talk']</t>
         </is>
       </c>
       <c r="L17" t="inlineStr"/>
@@ -1820,7 +1820,7 @@
       <c r="P17" t="inlineStr"/>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>https://github.com/shoot649854/IMG_DB/blob/main/profile.webp</t>
+          <t>https://raw.githubusercontent.com/shoot649854/IMG_DB/main/profile.webp</t>
         </is>
       </c>
       <c r="R17" t="inlineStr">
@@ -1842,7 +1842,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Published</t>
+          <t>Draft</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -1852,22 +1852,22 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>8</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>【Note】Procedures for using different ssh connection settings (config) with multiple Github accounts</t>
+          <t>Commonly Used React HooksGithub accounts</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>When working with multiple GitHub accounts, it's crucial to configure SSH connection settings properly to ensure seamless authentication. Here are the steps to set up and manage multiple SSH configurations</t>
+          <t>List of commonly used React hooks with brief explanations.</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Different_ssh_settings</t>
+          <t>React_Hooks</t>
         </is>
       </c>
       <c r="G18" s="2" t="n">
@@ -1900,7 +1900,7 @@
       <c r="P18" t="inlineStr"/>
       <c r="Q18" t="inlineStr">
         <is>
-          <t>https://github.com/shoot649854/IMG_DB/blob/main/profile.webp</t>
+          <t>https://raw.githubusercontent.com/shoot649854/IMG_DB/main/profile.webp</t>
         </is>
       </c>
       <c r="R18" t="inlineStr">
@@ -1914,6 +1914,86 @@
         </is>
       </c>
       <c r="T18" t="inlineStr">
+        <is>
+          <t>[{'icon': 'fab fa-linkedin', 'url': 'https://www.linkedin.com/in/shoto-morisaki-93b0a71bb/'}, {'icon': 'fab fa-github', 'url': 'https://github.com/shoot649854/'}, {'icon': 'fab fa-portfolio', 'url': 'https://portfolio-shoto.vercel.app/'}]</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Published</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Article</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>【Note】Procedures for using different ssh connection settings (config) with multiple Github accounts</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>When working with multiple GitHub accounts, it's crucial to configure SSH connection settings properly to ensure seamless authentication. Here are the steps to set up and manage multiple SSH configurations</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Different_ssh_settings</t>
+        </is>
+      </c>
+      <c r="G19" s="2" t="n">
+        <v>45333</v>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>Shoto Morisaki</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>sample/opened-laptop.jpg</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>Coding</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>['Git']</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr"/>
+      <c r="M19" t="inlineStr"/>
+      <c r="N19" t="inlineStr"/>
+      <c r="O19" t="inlineStr"/>
+      <c r="P19" t="inlineStr"/>
+      <c r="Q19" t="inlineStr">
+        <is>
+          <t>https://raw.githubusercontent.com/shoot649854/IMG_DB/main/profile.webp</t>
+        </is>
+      </c>
+      <c r="R19" t="inlineStr">
+        <is>
+          <t>Computer Science - University of California Santa Cruz | Intern - LiNK</t>
+        </is>
+      </c>
+      <c r="S19" t="inlineStr">
+        <is>
+          <t>Shoto Morisaki</t>
+        </is>
+      </c>
+      <c r="T19" t="inlineStr">
         <is>
           <t>[{'icon': 'fab fa-linkedin', 'url': 'https://www.linkedin.com/in/shoto-morisaki-93b0a71bb/'}, {'icon': 'fab fa-github', 'url': 'https://github.com/shoot649854/'}, {'icon': 'fab fa-portfolio', 'url': 'https://portfolio-shoto.vercel.app/'}]</t>
         </is>

</xml_diff>